<commit_message>
SD-68035 - CCRU - KPI Template fix
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC QSR.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC QSR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="QSR" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,6 +18,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">QSR!$A$1:$AM$48</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">QSR!$A$1:$AM$48</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">QSR!$A$1:$AM$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">QSR!$A$1:$AM$48</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1089,49 +1090,49 @@
   </sheetPr>
   <dimension ref="A1:AM48"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="60.2024291497976"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="93.6234817813765"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="60.7368421052632"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="94.4777327935223"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.1740890688259"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="108.404858299595"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="80.2307692307692"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="109.368421052632"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="80.8744939271255"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="1" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="1" width="6.96356275303644"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="24.6356275303644"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="22.0647773279352"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="1" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="59.0242914979757"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="59.4493927125506"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="36" min="36" style="1" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="37" min="37" style="1" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="38" min="38" style="1" width="10.6032388663968"/>
@@ -3348,7 +3349,9 @@
         <v>65</v>
       </c>
       <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
+      <c r="J29" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
       <c r="M29" s="6" t="s">

</xml_diff>